<commit_message>
Update Pertanggal 17 Januari 2023 13:48 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/SQL Generator/Data Initial/SysConfig.TblAppObject_MenuGroup.xlsx
+++ b/Documentation/Documents/SQL Generator/Data Initial/SysConfig.TblAppObject_MenuGroup.xlsx
@@ -436,13 +436,13 @@
   <dimension ref="B1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="2.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="14" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="2.42578125" style="1" customWidth="1"/>

</xml_diff>

<commit_message>
Update Pertanggal 27 Februari 2024 13:25 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/SQL Generator/Data Initial/SysConfig.TblAppObject_MenuGroup.xlsx
+++ b/Documentation/Documents/SQL Generator/Data Initial/SysConfig.TblAppObject_MenuGroup.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Main" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>SYS_PID</t>
   </si>
@@ -50,6 +50,39 @@
   </si>
   <si>
     <t>Name</t>
+  </si>
+  <si>
+    <t>IconSource</t>
+  </si>
+  <si>
+    <t>fas fa-home</t>
+  </si>
+  <si>
+    <t>fas fa-shopping-basket</t>
+  </si>
+  <si>
+    <t>fas fa-users</t>
+  </si>
+  <si>
+    <t>fas fa-credit-card</t>
+  </si>
+  <si>
+    <t>fas fa-chart-line</t>
+  </si>
+  <si>
+    <t>fas fa-hourglass-start</t>
+  </si>
+  <si>
+    <t>fas fa-cart-arrow-down</t>
+  </si>
+  <si>
+    <t>fas fa-warehouse</t>
+  </si>
+  <si>
+    <t>fas fa-registered</t>
+  </si>
+  <si>
+    <t>fas fa-user</t>
   </si>
 </sst>
 </file>
@@ -441,148 +474,182 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F11"/>
+  <dimension ref="B1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="2.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="2.42578125" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="3" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.42578125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="4">
+      <c r="C2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="4">
         <v>254000000000001</v>
       </c>
-      <c r="F2" s="7" t="str">
-        <f>CONCATENATE("PERFORM ""SchSysConfig"".""Func_TblAppObject_MenuGroup_SET""(varSystemLoginSession, null, null, null, varInstitutionBranchID, varBaseCurrencyID, '", B2, "'::varchar);")</f>
-        <v>PERFORM "SchSysConfig"."Func_TblAppObject_MenuGroup_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, varBaseCurrencyID, 'Home'::varchar);</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G2" s="7" t="str">
+        <f>CONCATENATE("PERFORM ""SchSysConfig"".""Func_TblAppObject_MenuGroup_SET""(varSystemLoginSession, null, null, null, varInstitutionBranchID, varBaseCurrencyID, '", B2, "'::varchar, '", C2, "'::varchar);")</f>
+        <v>PERFORM "SchSysConfig"."Func_TblAppObject_MenuGroup_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, varBaseCurrencyID, 'Home'::varchar, 'fas fa-home'::varchar);</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="4">
+      <c r="C3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="4">
         <v>254000000000002</v>
       </c>
-      <c r="F3" s="7" t="str">
-        <f t="shared" ref="F3:F11" si="0">CONCATENATE("PERFORM ""SchSysConfig"".""Func_TblAppObject_MenuGroup_SET""(varSystemLoginSession, null, null, null, varInstitutionBranchID, varBaseCurrencyID, '", B3, "'::varchar);")</f>
-        <v>PERFORM "SchSysConfig"."Func_TblAppObject_MenuGroup_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, varBaseCurrencyID, 'Budget'::varchar);</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G3" s="7" t="str">
+        <f t="shared" ref="G3:G11" si="0">CONCATENATE("PERFORM ""SchSysConfig"".""Func_TblAppObject_MenuGroup_SET""(varSystemLoginSession, null, null, null, varInstitutionBranchID, varBaseCurrencyID, '", B3, "'::varchar, '", C3, "'::varchar);")</f>
+        <v>PERFORM "SchSysConfig"."Func_TblAppObject_MenuGroup_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, varBaseCurrencyID, 'Budget'::varchar, 'fas fa-shopping-basket'::varchar);</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="4">
+      <c r="C4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="4">
         <v>254000000000003</v>
       </c>
-      <c r="F4" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>PERFORM "SchSysConfig"."Func_TblAppObject_MenuGroup_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, varBaseCurrencyID, 'Human Resource'::varchar);</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G4" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>PERFORM "SchSysConfig"."Func_TblAppObject_MenuGroup_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, varBaseCurrencyID, 'Human Resource'::varchar, 'fas fa-users'::varchar);</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="4">
+      <c r="C5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="4">
         <v>254000000000004</v>
       </c>
-      <c r="F5" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>PERFORM "SchSysConfig"."Func_TblAppObject_MenuGroup_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, varBaseCurrencyID, 'Finance'::varchar);</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G5" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>PERFORM "SchSysConfig"."Func_TblAppObject_MenuGroup_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, varBaseCurrencyID, 'Finance'::varchar, 'fas fa-credit-card'::varchar);</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="4">
+      <c r="C6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="4">
         <v>254000000000005</v>
       </c>
-      <c r="F6" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>PERFORM "SchSysConfig"."Func_TblAppObject_MenuGroup_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, varBaseCurrencyID, 'Sales'::varchar);</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G6" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>PERFORM "SchSysConfig"."Func_TblAppObject_MenuGroup_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, varBaseCurrencyID, 'Sales'::varchar, 'fas fa-chart-line'::varchar);</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="4">
+      <c r="C7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="4">
         <v>254000000000006</v>
       </c>
-      <c r="F7" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>PERFORM "SchSysConfig"."Func_TblAppObject_MenuGroup_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, varBaseCurrencyID, 'Process'::varchar);</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G7" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>PERFORM "SchSysConfig"."Func_TblAppObject_MenuGroup_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, varBaseCurrencyID, 'Process'::varchar, 'fas fa-hourglass-start'::varchar);</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="4">
+      <c r="C8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="4">
         <v>254000000000007</v>
       </c>
-      <c r="F8" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>PERFORM "SchSysConfig"."Func_TblAppObject_MenuGroup_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, varBaseCurrencyID, 'Purchase'::varchar);</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G8" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>PERFORM "SchSysConfig"."Func_TblAppObject_MenuGroup_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, varBaseCurrencyID, 'Purchase'::varchar, 'fas fa-cart-arrow-down'::varchar);</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="4">
+      <c r="C9" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="4">
         <v>254000000000008</v>
       </c>
-      <c r="F9" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>PERFORM "SchSysConfig"."Func_TblAppObject_MenuGroup_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, varBaseCurrencyID, 'Inventory'::varchar);</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G9" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>PERFORM "SchSysConfig"."Func_TblAppObject_MenuGroup_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, varBaseCurrencyID, 'Inventory'::varchar, 'fas fa-warehouse'::varchar);</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B10" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="4">
+      <c r="C10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="4">
         <v>254000000000009</v>
       </c>
-      <c r="F10" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>PERFORM "SchSysConfig"."Func_TblAppObject_MenuGroup_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, varBaseCurrencyID, 'Register'::varchar);</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G10" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>PERFORM "SchSysConfig"."Func_TblAppObject_MenuGroup_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, varBaseCurrencyID, 'Register'::varchar, 'fas fa-registered'::varchar);</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="4">
+      <c r="C11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="4">
         <v>254000000000010</v>
       </c>
-      <c r="F11" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>PERFORM "SchSysConfig"."Func_TblAppObject_MenuGroup_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, varBaseCurrencyID, 'Admin'::varchar);</v>
+      <c r="G11" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>PERFORM "SchSysConfig"."Func_TblAppObject_MenuGroup_SET"(varSystemLoginSession, null, null, null, varInstitutionBranchID, varBaseCurrencyID, 'Admin'::varchar, 'fas fa-user'::varchar);</v>
       </c>
     </row>
   </sheetData>

</xml_diff>